<commit_message>
Fixed bug that was adding the line numbers together twice
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kieran/Documents/Projects/CSCI318/csci318/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
   </bookViews>
   <sheets>
-    <sheet name="Google" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Bing" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Youdao" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Google" sheetId="1" r:id="rId1"/>
+    <sheet name="Bing" sheetId="2" r:id="rId2"/>
+    <sheet name="Youdao" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="179">
   <si>
     <t>The name bugleweed is a common name which can refer to several unrelated plants:.</t>
   </si>
@@ -153,6 +166,141 @@
     <t>Naturwolfen (Proteles cristata) är ett litet, insektsdödande däggdjur, infödt i Öst och Sydafrika.</t>
   </si>
   <si>
+    <t>Wahoo (Acanthocybium solandri) is a scombrid fish found worldwide in tropical and subtropical seas.</t>
+  </si>
+  <si>
+    <t>Wahoo（Acanthocybium solandri）是全球热带和亚热带海域发现的scombrid鱼。</t>
+  </si>
+  <si>
+    <t>Wahoo（Acanthocybium solandri）は、熱帯および亜熱帯の海域で世界中で発見された種間魚です。</t>
+  </si>
+  <si>
+    <t>Wahoo (Acanthocybium solandri)는 열대 및 아열대 바다에서 전 세계적으로 발견되는 바지락 물고기입니다.</t>
+  </si>
+  <si>
+    <t>Wahoo (Acanthocybium solandri) est un poisson scombrid trouvé dans le monde entier dans les mers tropicales et subtropicales.</t>
+  </si>
+  <si>
+    <t>Wahoo (Acanthocybium solandri) - это мохнатая рыба, найденная во всем мире в тропических и субтропических морях.</t>
+  </si>
+  <si>
+    <t>Wahoo (Acanthocybium solandri) é um peixe scombrid encontrado mundialmente em mares tropicais e subtropicais.</t>
+  </si>
+  <si>
+    <t>Wahoo (Acanthocybium solandri) es un pez scombrid encontrado en todo el mundo en mares tropicales y subtropicales.</t>
+  </si>
+  <si>
+    <t>Wahoo (Acanthocybium solandri) är en scombrid fisk som finns över hela världen i tropiska och subtropiska hav.</t>
+  </si>
+  <si>
+    <t>An accident, also known as an unintentional injury, is an undesirable, incidental, and unplanned event that could have been prevented had circumstances leading up to the accident been recognized, and acted upon, prior to its occurrence.</t>
+  </si>
+  <si>
+    <t>事故也被称为无意伤害事件，是一种不可预料的，偶然的和计划外的事件，如果在发生事故之前已经认识到并采取行动，可能会发生事故。</t>
+  </si>
+  <si>
+    <t>意図しない傷害としても知られる事故は、発生前に事故に至った状況が認識され、遂行された場合に、予防できなかった望ましくない、偶発的で計画外の事象である。</t>
+  </si>
+  <si>
+    <t>의도하지 않은 상해라고도하는 사고는 바람직하지 않은 우발적 인 계획되지 않은 사건으로서 사고까지의 상황을 인식하고 발생시킨 후에 예방할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>Un accident, également connu sous le nom de blessure involontaire, est un événement indésirable, fortuit et imprévu qui aurait pu être évité si les circonstances menant à l&amp;#39;accident avaient été reconnues et mises en pratique avant son apparition.</t>
+  </si>
+  <si>
+    <t>Авария, также известная как непреднамеренная травма, является нежелательным, случайным и незапланированным событием, которое могло быть предотвращено, если бы обстоятельства, приведшие к аварии, были признаны и действовали до его возникновения.</t>
+  </si>
+  <si>
+    <t>Um acidente, também conhecido como lesão involuntária, é um evento indesejável, incidental e não planejado que poderia ter sido impedido se as circunstâncias que conduzissem ao acidente fossem reconhecidas e atuadas antes da ocorrência.</t>
+  </si>
+  <si>
+    <t>Un accidente, también conocido como una lesión no intencional, es un evento indeseable, incidental y no planificado que podría haberse evitado si las circunstancias que condujeron al accidente hubiesen sido reconocidas y actuadas antes de su ocurrencia.</t>
+  </si>
+  <si>
+    <t>En olycka, även känd som en oavsiktlig skada, är en oönskad, tillfällig och oförutsedd händelse som skulle ha kunnat förebyggas om omständigheter som ledde fram till olyckan hade erkänts och agerats före dess förekomst.</t>
+  </si>
+  <si>
+    <t>Accompaniment is the musical parts which provide the rhythmic and/or harmonic support for the melody or main themes of a song or instrumental piece.</t>
+  </si>
+  <si>
+    <t>伴奏是为歌曲或乐器的旋律或主要主题提供节奏和/或谐波支持的音乐部分。</t>
+  </si>
+  <si>
+    <t>伴奏は、曲や楽器のメロディやメインテーマのリズムやハーモニックのサポートを提供する音楽パートです。</t>
+  </si>
+  <si>
+    <t>반주는 멜로디 또는 노래 또는 악기 부분의 주요 테마에 대한 리듬 및 / 또는 고조파 지원을 제공하는 음악 파트입니다.</t>
+  </si>
+  <si>
+    <t>L&amp;#39;accompagnement est les parties musicales qui apportent le support rythmique et / ou harmonique à la mélodie ou aux thèmes principaux d&amp;#39;une chanson ou d&amp;#39;une pièce instrumentale.</t>
+  </si>
+  <si>
+    <t>Аккомпанемент - это музыкальные части, которые обеспечивают ритмическую и / или гармоническую поддержку мелодии или основных тем песни или инструментальной пьесы.</t>
+  </si>
+  <si>
+    <t>Acompanhamento são as peças musicais que fornecem o suporte rítmico e / ou harmônico para a melodia ou temas principais de uma música ou peça instrumental.</t>
+  </si>
+  <si>
+    <t>Acompañamiento son las partes musicales que proporcionan el apoyo rítmico y / o armónico para la melodía o temas principales de una canción o pieza instrumental.</t>
+  </si>
+  <si>
+    <t>Accompaniment är de musikaliska delarna som ger det rytmiska och / eller harmoniska stödet för melodin eller huvudteman i en sång eller instrumentell del.</t>
+  </si>
+  <si>
+    <t>"From each according to his ability, to each according to his needs" (French: De chacun selon ses moyens, à chacun selon ses besoins; German: Jeder nach seinen Fähigkeiten, jedem nach seinen Bedürfnissen) is a slogan popularised by Karl Marx in his 1875 Critique of the Gotha Program.</t>
+  </si>
+  <si>
+    <t>（法语：De chacun selon ses moyens，àchacun selon ses besoins;德语：Jeder nach seinenFähigkeiten，jedem nach seinenBedürfnissen）是卡尔·马克思（Karl Marx）普及的口号，他的1875年哥达计划批评。</t>
+  </si>
+  <si>
+    <t>「彼の能力に応じて、それぞれのニーズに応じて」（フランス語：De Chacun selon ses mesens、Čacunselon ses besoins、ドイツ語：Jeder nach seinenFähigkeiten、jedem nach seinenBedürfnissen）は、Karl Marxによって大衆化されたスローガンです。彼の1875年のGothaプログラム批判。</t>
+  </si>
+  <si>
+    <t>&amp;quot;자신의 능력에 따라 각자 자신의 필요에 따라&amp;quot;(프랑스어 : De Chacun selon ses mesens, à chacun selon ses besoins, 독일어 : Jeder nach seinen Fähigkeiten, jedem nach seinen Bedürfnissen)는 Karl Marx에서 대중화 된 슬로건이다. 그의 1875 고타 프로그램 비판.</t>
+  </si>
+  <si>
+    <t>«De chacun selon ses capacités, à chacun selon ses besoins» est un slogan popularisé par Karl Marx dans «Le Monde de la Terre». sa critique de 1875 du programme Gotha.</t>
+  </si>
+  <si>
+    <t>«От каждого по его способностям, каждому по его потребностям» (французский язык: «De chacun selon ses moyens», «chacun selon ses besoins», немецкий: Jeder nach seinen Fähigkeiten, jedem nach seinen Bedürfnissen) - это лозунг, популяризированный Карлом Маркс в его Критика Готской программы 1875 года.</t>
+  </si>
+  <si>
+    <t>&amp;quot;De cada um segundo a sua capacidade, para cada um de acordo com suas necessidades&amp;quot; (French: De chacun selon ses moyens, a critério dos candidatos, alemão: Jeder nach seinen Fähigkeiten, jedem nach seinen Bedürfnissen) é um slogan popularizado por Karl Marx em sua Crítica de 1875 sobre o programa de Gotha.</t>
+  </si>
+  <si>
+    <t>&amp;quot;De cada uno de acuerdo a su capacidad, a cada uno de acuerdo a sus necesidades&amp;quot; (francés: De chacun selon ses moyens, à chacun selon ses besoins) es un eslogan popularizado por Karl Marx en su Crítica 1875 del Programa de Gotha.</t>
+  </si>
+  <si>
+    <t>&amp;quot;Från varje enligt hans förmåga, till var och en enligt hans behov&amp;quot; (franska: De chacun selon ses moyens, en chacun selon ses besoins, tyska: Jeder nach seinen Fähigkeiten, jedem nach seinen Bedürfnissen) är en slogan populär av Karl Marx i hans 1875 kritik av Gotha-programmet.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata is a tropical fruit-bearing shrub or small tree in the family Malpighiaceae.</t>
+  </si>
+  <si>
+    <t>马鞭草属（Malpighia emarginata）是马鞭草科的一种热带水果灌木或小树。</t>
+  </si>
+  <si>
+    <t>Malpighia emarginataは、Malpighiaceae科の熱帯の果実を持つ低木または小さな木です。</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata는 열대 과일 보유 관목이나 Malpighiaceae 계통의 작은 나무입니다.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata est un arbuste à fruits tropicaux ou un petit arbre de la famille des Malpighiaceae.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata - тропический фруктовый кустарник или небольшое дерево в семье Malpighiaceae.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata é um arbusto frutífero tropical ou pequena árvore na família Malpighiaceae.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata es un arbusto o árbol pequeño frutal tropical en la familia Malpighiaceae.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata är en tropisk fruktbärande buske eller litet träd i familjen Malpighiaceae.</t>
+  </si>
+  <si>
     <t>名称夏枯草是一个共同的名字，这可以指几个不相关的植物:。</t>
   </si>
   <si>
@@ -273,6 +421,123 @@
     <t>Aardwolf (Proteles cristata) är en liten, insektsätande däggdjur, infödda till östra och södra Afrika.</t>
   </si>
   <si>
+    <t>刺鲅 (Acanthocybium solandri) 是鲭科鱼，产于世界各地的热带和亚热带海域。</t>
+  </si>
+  <si>
+    <t>ワフー (Acanthocybium solandri) は世界中で見られる熱帯・亜熱帯の海で発見された魚です。</t>
+  </si>
+  <si>
+    <t>와 후 (Acanthocybium solandri)는 전세계 열 대와 아열대 바다에서 발견 scombrid 물고기입니다.</t>
+  </si>
+  <si>
+    <t>Wahoo (Acanthocybium solandri) est un poisson scombrid dans le monde entier dans les mers tropicales et subtropicales.</t>
+  </si>
+  <si>
+    <t>Ваху (Acanthocybium solandri) является scombrid рыбы, нашли по всему миру в тропических и субтропических водах.</t>
+  </si>
+  <si>
+    <t>Wahoo (Acanthocybium solandri) é um peixe de scombrid encontrado em todo o mundo em mares tropicais e subtropicais.</t>
+  </si>
+  <si>
+    <t>Peto (Acanthocybium solandri) es un pez de escómbridos encontrado en todo el mundo en mares tropicales y subtropicales.</t>
+  </si>
+  <si>
+    <t>Wahoo (Acanthocybium solandri) är en scombrid fisk finns över hela världen i tropiska och subtropiska hav.</t>
+  </si>
+  <si>
+    <t>一次事故，也被称为非故意的伤害，是不可取的偶然的和本来可以避免的意外的事件已经导致被公认，和付诸实行之前，对其发生的意外情况。</t>
+  </si>
+  <si>
+    <t>として知られている非意図的傷害、事故は防げた可能性があります予期しないイベントが認識、その発生を事前に行動をされて事故に至るまでの状況、望ましくない、偶発的、です。</t>
+  </si>
+  <si>
+    <t>로 알려진 또한 의도 하지 않은 부상, 사고는 바람직하지 않은, 부수적, 그리고 예기치 않은 이벤트를 막을 수 했다 상황 인식, 그리고 시 행동, 그 발생 하기 전에 사고로 이어지는.</t>
+  </si>
+  <si>
+    <t>Un accident, également connu sous le nom d’une blessure accidentelle, est un accessoire peu souhaitable, et événement imprévu qui aurait pu être évitée si les circonstances menant à l’accident, été reconnue et a agi à, avant son apparition.</t>
+  </si>
+  <si>
+    <t>Аварии, также известный как непреднамеренных травм, является нежелательным, случайный, и незапланированные события, которое можно было бы предотвратить было обстоятельств, приведших к аварии было признанным и действовал по, до ее возникновения.</t>
+  </si>
+  <si>
+    <t>Um acidente, também conhecido como uma lesão não intencional, é acidental indesejável, e eventos não planejados que poderiam ter sido evitados tinham circunstâncias que antecederam o acidente foi reconhecido e agiu em cima, antes da sua ocorrência.</t>
+  </si>
+  <si>
+    <t>Un accidente, también conocida como una lesión accidental, es indeseable, fortuito y evento imprevisto que podría haberse evitado circunstancias que precedieron al accidente ha reconocido y actuado sobre, antes de su ocurrencia.</t>
+  </si>
+  <si>
+    <t>En olycka, även känd som en oavsiktlig skada, är en oönskad, oförutsedda och oplanerad händelse som kunde ha förhindrats hade omständigheter som ledde fram till olyckan varit erkänd, och agerade vid, före dess förekomst.</t>
+  </si>
+  <si>
+    <t>伴奏是提供的节奏和/或谐波的音乐部分支持的旋律或主题的歌曲或乐曲。</t>
+  </si>
+  <si>
+    <t>伴奏は、リズムや高調波を提供する音楽的な部品をメロディーや曲やインストゥルメンタル作品の主要なテーマのサポートです。</t>
+  </si>
+  <si>
+    <t>반주 리듬 또는 고조파는 음악 부분 멜로디 또는 노래나 기 악 작품의 주요 테마에 대 한 지원 이다.</t>
+  </si>
+  <si>
+    <t>Accompagnement, c’est les parties musicales qui assurent la rythmique ou harmonique soutiennent pour la mélodie ou les thèmes principaux d’une chanson ou une pièce instrumentale.</t>
+  </si>
+  <si>
+    <t>Сопровождение – музыкальных частей, которые обеспечивают художественной и/или гармонические поддержку мелодию или основные темы песни или инструментальная пьеса.</t>
+  </si>
+  <si>
+    <t>Acompanhamento é que as peças musicais que fornecem a rítmica e/ou harmônica oferece suporte para a melodia ou os temas principais de uma canção ou uma peça instrumental.</t>
+  </si>
+  <si>
+    <t>Acompañamiento es soporte de las piezas musicales que la rítmica o armónica de la melodía o temas principales de una canción o pieza instrumental.</t>
+  </si>
+  <si>
+    <t>Ackompanjemang är de musikaliska delar som sörjer den rytmiska och harmoniska stöd för melodi eller huvudteman i en låt eller ett instrumentalt stycke.</t>
+  </si>
+  <si>
+    <t>"从每个根据他的能力，做到各尽所能需要"(法语： De chacun 承认 ses 乘坐、 à chacun se 来满足其承认;德国： Jeder 代表了青年 jedem 代表了青年 Bedürfnissen Fähigkeiten) 一句口号卡尔 · 马克思在哥达纲领他 1875年批判普及开来。</t>
+  </si>
+  <si>
+    <t>「彼の能力に従ってそれぞれから彼によるとそれぞれにニーズ」(フランス語: De 映画 selon ses moyens、アラカルト映画 selon ses besoins;ドイツ語: Jeder nach 青年の nach 青年 Bedürfnissen Fähigkeiten) 1875 Gotha プログラムの批評でカール ・ マルクスによって大衆のキャロルルイス スローガンです。</t>
+  </si>
+  <si>
+    <t>"각 그의 능력에 따라, 그에 따라 각 필요" (프랑스어: 데 모두가 따르면 ses moyens, 일품 모두가 따르면 ses의; 독일: 어느 nach seinen Fähigkeiten, jedem에 seinen Bedürfnissen)는 슬로건 타 프로그램의 그의 1875 비판에 Karl Marx에 의해 유명해 졌.</t>
+  </si>
+  <si>
+    <t>« De chacun selon ses capacités, à chacun selon ses besoins » (Français : De chacun selon ses moyens, à chacun selon ses besoins ; Allemand : Jeder nach seinen Fähigkeiten, jedem nach seinen frische) est un slogan popularisé par Karl Marx dans sa Critique de 1875 du programme de Gotha.</t>
+  </si>
+  <si>
+    <t>«От каждого по способностям, каждому по его потребностей» (французский: De chacun согласно ses средства, меню chacun согласно ses нужд; Немецкий: Jeder nach сэйнэн Fähigkeiten, jedem nach сэйнэн Bedürfnissen) является популярным лозунг Карл Маркс в своем 1875 критика Гота программы.</t>
+  </si>
+  <si>
+    <t>"De cada um de acordo com sua capacidade, a cada um segundo a sua precisa" (francês: De chacun selon ses moyens, à chacun selon ses besoins; Alemão: Jeder nach seinen Fähigkeiten, Jed nach seinen Bedürfnissen) é um slogan popularizado por Karl Marx em sua crítica de 1875, do programa de Gotha.</t>
+  </si>
+  <si>
+    <t>"De cada uno según su capacidad, a cada uno según sus necesidades" (Francés: De chacun selon ses moyens, à chacun selon ses besoins; Alemán: Jeder nach seinen Fähigkeiten, jedem nach seinen Bedürfnissen) es un lema popularizado por Karl Marx en su crítica del programa de Gotha de 1875.</t>
+  </si>
+  <si>
+    <t>”Från var och en efter hans förmåga, till var och en efter hans behov” (franska: De chacun selon ses moyens, à chacun selon ses besoins; Tyska: Jeder nach förmedla Fähigkeiten, jedem nach förmedla Bedürfnissen) är en slogan som populariserade av Karl Marx i sin 1875 kritik av programmet Gotha.</t>
+  </si>
+  <si>
+    <t>金虎尾 emarginata 是热带果实的灌木或小乔木在家庭 Malpighiaceae。</t>
+  </si>
+  <si>
+    <t>生の発生経過、熱帯果実軸受低木または家族キントラノオ科の小さなツリーです。</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata는 열 대 과일 베어링 나무 또는 가족 Malpighiaceae에에서 작은 나무.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata est un arbuste tropical de fruitiers ou un petit arbre de la famille des Malpighiaceae.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata — тропических фруктовых кустарник или небольшое дерево семейства Мальпигиевые.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata é um tropical frutíferas arbusto ou pequena árvore da família Malpighiaceae.</t>
+  </si>
+  <si>
+    <t>Malpighia emarginata es una tropical frutal arbusto o árbol pequeño de la familia Malpighiaceae.</t>
+  </si>
+  <si>
     <t>“bugleweed”这个名字是一个常见的名字，可以指几个不相关的植物。</t>
   </si>
   <si>
@@ -286,25 +551,39 @@
   </si>
   <si>
     <t>土狼(Proteles cristata)是一种小型的食虫哺乳动物，原产于非洲东部和南部。</t>
+  </si>
+  <si>
+    <t>Wahoo(acanthcybium solandri)是一种在全球热带和亚热带海域发现的scombrid鱼。</t>
+  </si>
+  <si>
+    <t>一场意外事故，也被称为无意伤害，是一种不受欢迎的、偶然的、意外的事件，如果在事故发生前发生事故，并在事故发生前采取行动，就可以防止事故发生。</t>
+  </si>
+  <si>
+    <t>伴奏是为歌曲或乐器的旋律或主要主题提供有节奏和/或和声支持的音乐部分。</t>
+  </si>
+  <si>
+    <t>“根据他的能力，根据他的需要，每一个人”(法语:De chacun selon ses moyens,chacun selon ses besoins;德语:Jeder nach seinen Fahigkeiten,jedem nach seinen Bedurfnissen)是卡尔·马克思在他1875年对Gotha计划的批判中广为流传的一个口号。</t>
+  </si>
+  <si>
+    <t>马皮吉亚(Malpighia emarginata)是一种热带灌木或小乔木，生长在malpighi科。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -320,15 +599,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -616,20 +901,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -658,7 +939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -687,7 +968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -716,7 +997,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -745,7 +1026,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -774,335 +1055,762 @@
         <v>44</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A12" sqref="A12:V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="H4" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="F5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>81</v>
       </c>
-      <c r="G5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" t="s">
-        <v>84</v>
+      <c r="B10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="H4" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="B5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" t="s">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" t="s">
-        <v>84</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>